<commit_message>
docs baru dari client
</commit_message>
<xml_diff>
--- a/docs/Daftar API dan Dummy Data.xlsx
+++ b/docs/Daftar API dan Dummy Data.xlsx
@@ -2457,16 +2457,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>1726407</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>166688</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>154781</xdr:rowOff>
+      <xdr:rowOff>178593</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>330995</xdr:colOff>
+      <xdr:colOff>509588</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>689821</xdr:rowOff>
+      <xdr:rowOff>713633</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2489,7 +2489,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6988970" y="154781"/>
+          <a:off x="7465219" y="178593"/>
           <a:ext cx="10058400" cy="5499946"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2791,8 +2791,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16:E17"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3475,7 +3475,7 @@
   <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4511,8 +4511,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W44"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5841,8 +5841,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:DB158"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="L69" sqref="L69"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23363,7 +23363,7 @@
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24601,7 +24601,7 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="G2" sqref="G2:G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25050,8 +25050,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G1007"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33454,8 +33454,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33851,8 +33851,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z42"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27:F29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
perbaikan pada calling api sakernas_api
</commit_message>
<xml_diff>
--- a/docs/Daftar API dan Dummy Data.xlsx
+++ b/docs/Daftar API dan Dummy Data.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Project Coding\Web\Node\sakernas\docs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="195" windowWidth="20115" windowHeight="7875" tabRatio="861"/>
+    <workbookView xWindow="240" yWindow="195" windowWidth="20115" windowHeight="7875" tabRatio="861" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="List API" sheetId="13" r:id="rId1"/>
@@ -2405,6 +2410,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -2545,7 +2553,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2580,7 +2588,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2791,7 +2799,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
@@ -2805,7 +2813,7 @@
     <col min="6" max="16384" width="9.140625" style="31"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1" s="32" t="s">
         <v>527</v>
       </c>
@@ -2932,7 +2940,7 @@
         <v>721</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B13" s="31" t="s">
         <v>613</v>
       </c>
@@ -23737,7 +23745,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8:F10"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23856,8 +23864,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33851,8 +33859,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>